<commit_message>
1) Updating unit test coverage to verify handling of blank cells. 2) Updating RELEASE_NOTES.md in preparation for publishing another version to NuGet
</commit_message>
<xml_diff>
--- a/tests/ExcelProvider.Tests/DataTypes.xlsx
+++ b/tests/ExcelProvider.Tests/DataTypes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\Documents\GitHub\fsharpx\tests\FSharpx.TypeProviders.Excel.Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\Personal\ExcelProvider\tests\ExcelProvider.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -48,12 +48,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,18 +87,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,16 +405,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -436,16 +448,21 @@
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <f ca="1">NOW()</f>
-        <v>41449.359279166667</v>
+        <v>41640</v>
       </c>
       <c r="E2" s="4">
-        <f ca="1" xml:space="preserve"> NOW()</f>
-        <v>41449.359279166667</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F2" s="5">
         <v>100</v>
       </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>